<commit_message>
change plan to build this website
</commit_message>
<xml_diff>
--- a/0_plan/task.xlsx
+++ b/0_plan/task.xlsx
@@ -1,48 +1,421 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="16155" windowHeight="8505"/>
+    <workbookView windowWidth="19740" windowHeight="8250" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="describe project" sheetId="1" r:id="rId1"/>
+    <sheet name="feature" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>chat</t>
+  </si>
+  <si>
+    <t>social media</t>
+  </si>
+  <si>
+    <t>recommend</t>
+  </si>
+  <si>
+    <t>destination</t>
+  </si>
+  <si>
+    <t>detail-destination</t>
+  </si>
+  <si>
+    <t>change-new-destination</t>
+  </si>
+  <si>
+    <t>self information</t>
+  </si>
+  <si>
+    <t>travel news</t>
+  </si>
+  <si>
+    <t>travel expreriend</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <family val="2"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="2"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -50,9 +423,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -61,10 +676,57 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -355,50 +1017,118 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" ht="19" customHeight="1"/>
+    <row r="2" ht="19" customHeight="1" spans="2:3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="19" customHeight="1" spans="3:3">
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" ht="19" customHeight="1" spans="3:3">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" ht="19" customHeight="1" spans="3:3">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" ht="19" customHeight="1" spans="3:3">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" ht="19" customHeight="1" spans="3:3">
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" ht="19" customHeight="1" spans="3:3">
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" ht="19" customHeight="1" spans="3:3">
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" ht="19" customHeight="1" spans="3:3">
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" ht="19" customHeight="1" spans="3:3">
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" ht="19" customHeight="1"/>
+    <row r="13" ht="19" customHeight="1"/>
+    <row r="14" ht="19" customHeight="1"/>
+    <row r="15" ht="19" customHeight="1"/>
+    <row r="16" ht="19" customHeight="1"/>
+    <row r="17" ht="19" customHeight="1"/>
+    <row r="18" ht="19" customHeight="1"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs(plan): change plan, add ignore
</commit_message>
<xml_diff>
--- a/0_plan/task.xlsx
+++ b/0_plan/task.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19740" windowHeight="8250" activeTab="1"/>
+    <workbookView windowWidth="19740" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="describe project" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <t>chat</t>
   </si>
   <si>
-    <t>social media</t>
+    <t>social</t>
   </si>
   <si>
     <t>recommend</t>
@@ -48,7 +48,7 @@
     <t>travel news</t>
   </si>
   <si>
-    <t>travel expreriend</t>
+    <t>travel exprerience</t>
   </si>
 </sst>
 </file>
@@ -56,12 +56,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,38 +78,60 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -123,6 +145,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -132,92 +178,39 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -236,31 +229,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,7 +331,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -284,25 +379,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,103 +397,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,6 +414,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -439,15 +441,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -459,6 +452,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -480,26 +488,20 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -512,159 +514,150 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1025,8 +1018,8 @@
   <sheetPr/>
   <dimension ref="B1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -1104,8 +1097,8 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>

</xml_diff>